<commit_message>
Updated flownetwork.py and added iron.figs.ipynb
</commit_message>
<xml_diff>
--- a/data/raw/Steel_Scraps_Share_Crude_Steel_BIR.xlsx
+++ b/data/raw/Steel_Scraps_Share_Crude_Steel_BIR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faisal/Documents/iESD/input/iron/reading/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faisal/Documents/iESD/FeFlow/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C4F867-C29C-804E-966E-F1214CF1AB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79AB7A0-DD5F-4842-B727-0F79EB194B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="1500" windowWidth="27240" windowHeight="15940" activeTab="2" xr2:uid="{7F4D77FC-CD1F-4644-8536-C9A78727609B}"/>
   </bookViews>
@@ -5546,17 +5546,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="N28:O28"/>
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="N28:O28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5566,9 +5566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0D1D49-31BC-1740-BB33-8598D666CF4C}">
   <dimension ref="A1:T176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T136" sqref="T136"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12366,14 +12366,14 @@
         <v>6115</v>
       </c>
       <c r="R140" s="1">
-        <f>((J140+K140+L140)*100)/D140</f>
+        <f t="shared" ref="R140:R176" si="0">((J140+K140+L140)*100)/D140</f>
         <v>43.816254416961129</v>
       </c>
       <c r="S140">
         <v>2000</v>
       </c>
       <c r="T140">
-        <f>(R140/100) * D140</f>
+        <f t="shared" ref="T140:T160" si="1">(R140/100) * D140</f>
         <v>372</v>
       </c>
     </row>
@@ -12428,14 +12428,14 @@
         <v>6195</v>
       </c>
       <c r="R141" s="1">
-        <f>((J141+K141+L141)*100)/D141</f>
+        <f t="shared" si="0"/>
         <v>44.653349001175087</v>
       </c>
       <c r="S141">
         <v>2001</v>
       </c>
       <c r="T141">
-        <f>(R141/100) * D141</f>
+        <f t="shared" si="1"/>
         <v>380</v>
       </c>
     </row>
@@ -12490,14 +12490,14 @@
         <v>6274</v>
       </c>
       <c r="R142" s="1">
-        <f>((J142+K142+L142)*100)/D142</f>
+        <f t="shared" si="0"/>
         <v>44.358407079646021</v>
       </c>
       <c r="S142">
         <v>2002</v>
       </c>
       <c r="T142">
-        <f>(R142/100) * D142</f>
+        <f t="shared" si="1"/>
         <v>401.00000000000006</v>
       </c>
     </row>
@@ -12552,14 +12552,14 @@
         <v>6354</v>
       </c>
       <c r="R143" s="1">
-        <f>((J143+K143+L143)*100)/D143</f>
+        <f t="shared" si="0"/>
         <v>42.577319587628864</v>
       </c>
       <c r="S143">
         <v>2003</v>
       </c>
       <c r="T143">
-        <f>(R143/100) * D143</f>
+        <f t="shared" si="1"/>
         <v>413</v>
       </c>
     </row>
@@ -12614,14 +12614,14 @@
         <v>6433</v>
       </c>
       <c r="R144" s="1">
-        <f>((J144+K144+L144)*100)/D144</f>
+        <f t="shared" si="0"/>
         <v>42.857142857142854</v>
       </c>
       <c r="S144">
         <v>2004</v>
       </c>
       <c r="T144">
-        <f>(R144/100) * D144</f>
+        <f t="shared" si="1"/>
         <v>459</v>
       </c>
     </row>
@@ -12676,14 +12676,14 @@
         <v>6512</v>
       </c>
       <c r="R145" s="1">
-        <f>((J145+K145+L145)*100)/D145</f>
+        <f t="shared" si="0"/>
         <v>41.695804195804193</v>
       </c>
       <c r="S145">
         <v>2005</v>
       </c>
       <c r="T145">
-        <f>(R145/100) * D145</f>
+        <f t="shared" si="1"/>
         <v>476.99999999999994</v>
       </c>
     </row>
@@ -12738,14 +12738,14 @@
         <v>6592</v>
       </c>
       <c r="R146" s="1">
-        <f>((J146+K146+L146)*100)/D146</f>
+        <f t="shared" si="0"/>
         <v>41.058540497193263</v>
       </c>
       <c r="S146">
         <v>2006</v>
       </c>
       <c r="T146">
-        <f>(R146/100) * D146</f>
+        <f t="shared" si="1"/>
         <v>512</v>
       </c>
     </row>
@@ -12800,14 +12800,14 @@
         <v>6671</v>
       </c>
       <c r="R147" s="1">
-        <f>((J147+K147+L147)*100)/D147</f>
+        <f t="shared" si="0"/>
         <v>39.747399702823181</v>
       </c>
       <c r="S147">
         <v>2007</v>
       </c>
       <c r="T147">
-        <f>(R147/100) * D147</f>
+        <f t="shared" si="1"/>
         <v>535</v>
       </c>
     </row>
@@ -12862,14 +12862,14 @@
         <v>6750</v>
       </c>
       <c r="R148" s="1">
-        <f>((J148+K148+L148)*100)/D148</f>
+        <f t="shared" si="0"/>
         <v>40.632054176072238</v>
       </c>
       <c r="S148">
         <v>2008</v>
       </c>
       <c r="T148">
-        <f>(R148/100) * D148</f>
+        <f t="shared" si="1"/>
         <v>540</v>
       </c>
     </row>
@@ -12924,14 +12924,14 @@
         <v>6829</v>
       </c>
       <c r="R149" s="1">
-        <f>((J149+K149+L149)*100)/D149</f>
+        <f t="shared" si="0"/>
         <v>36.363636363636367</v>
       </c>
       <c r="S149">
         <v>2009</v>
       </c>
       <c r="T149">
-        <f>(R149/100) * D149</f>
+        <f t="shared" si="1"/>
         <v>448</v>
       </c>
     </row>
@@ -12986,14 +12986,14 @@
         <v>6909</v>
       </c>
       <c r="R150" s="1">
-        <f>((J150+K150+L150)*100)/D150</f>
+        <f t="shared" si="0"/>
         <v>38.108680310515176</v>
       </c>
       <c r="S150">
         <v>2010</v>
       </c>
       <c r="T150">
-        <f>(R150/100) * D150</f>
+        <f t="shared" si="1"/>
         <v>540</v>
       </c>
     </row>
@@ -13048,14 +13048,14 @@
         <v>6988</v>
       </c>
       <c r="R151" s="1">
-        <f>((J151+K151+L151)*100)/D151</f>
+        <f t="shared" si="0"/>
         <v>38.486842105263158</v>
       </c>
       <c r="S151">
         <v>2011</v>
       </c>
       <c r="T151">
-        <f>(R151/100) * D151</f>
+        <f t="shared" si="1"/>
         <v>585</v>
       </c>
     </row>
@@ -13110,14 +13110,14 @@
         <v>7067</v>
       </c>
       <c r="R152" s="1">
-        <f>((J152+K152+L152)*100)/D152</f>
+        <f t="shared" si="0"/>
         <v>37.797810688989053</v>
       </c>
       <c r="S152">
         <v>2012</v>
       </c>
       <c r="T152">
-        <f>(R152/100) * D152</f>
+        <f t="shared" si="1"/>
         <v>587</v>
       </c>
     </row>
@@ -13174,14 +13174,14 @@
         <v>7146</v>
       </c>
       <c r="R153" s="1">
-        <f>((J153+K153+L153)*100)/D153</f>
+        <f t="shared" si="0"/>
         <v>38.025477707006367</v>
       </c>
       <c r="S153">
         <v>2013</v>
       </c>
       <c r="T153">
-        <f>(R153/100) * D153</f>
+        <f t="shared" si="1"/>
         <v>597</v>
       </c>
     </row>
@@ -13238,14 +13238,14 @@
         <v>7225</v>
       </c>
       <c r="R154" s="1">
-        <f>((J154+K154+L154)*100)/D154</f>
+        <f t="shared" si="0"/>
         <v>38.272383354350566</v>
       </c>
       <c r="S154">
         <v>2014</v>
       </c>
       <c r="T154">
-        <f>(R154/100) * D154</f>
+        <f t="shared" si="1"/>
         <v>607</v>
       </c>
     </row>
@@ -13302,14 +13302,14 @@
         <v>7302</v>
       </c>
       <c r="R155" s="1">
-        <f>((J155+K155+L155)*100)/D155</f>
+        <f t="shared" si="0"/>
         <v>38.552713661883971</v>
       </c>
       <c r="S155">
         <v>2015</v>
       </c>
       <c r="T155">
-        <f>(R155/100) * D155</f>
+        <f t="shared" si="1"/>
         <v>618</v>
       </c>
     </row>
@@ -13366,14 +13366,14 @@
         <v>7379</v>
       </c>
       <c r="R156" s="1">
-        <f>((J156+K156+L156)*100)/D156</f>
+        <f t="shared" si="0"/>
         <v>38.827160493827158</v>
       </c>
       <c r="S156">
         <v>2016</v>
       </c>
       <c r="T156">
-        <f>(R156/100) * D156</f>
+        <f t="shared" si="1"/>
         <v>628.99999999999989</v>
       </c>
     </row>
@@ -13430,14 +13430,14 @@
         <v>7455</v>
       </c>
       <c r="R157" s="1">
-        <f>((J157+K157+L157)*100)/D157</f>
+        <f t="shared" si="0"/>
         <v>39.180929095354522</v>
       </c>
       <c r="S157">
         <v>2017</v>
       </c>
       <c r="T157">
-        <f>(R157/100) * D157</f>
+        <f t="shared" si="1"/>
         <v>641</v>
       </c>
     </row>
@@ -13494,14 +13494,14 @@
         <v>7529</v>
       </c>
       <c r="R158" s="1">
-        <f>((J158+K158+L158)*100)/D158</f>
+        <f t="shared" si="0"/>
         <v>39.443436176648518</v>
       </c>
       <c r="S158">
         <v>2018</v>
       </c>
       <c r="T158">
-        <f>(R158/100) * D158</f>
+        <f t="shared" si="1"/>
         <v>652</v>
       </c>
     </row>
@@ -13558,14 +13558,14 @@
         <v>7603</v>
       </c>
       <c r="R159" s="1">
-        <f>((J159+K159+L159)*100)/D159</f>
+        <f t="shared" si="0"/>
         <v>39.880239520958085</v>
       </c>
       <c r="S159">
         <v>2019</v>
       </c>
       <c r="T159">
-        <f>(R159/100) * D159</f>
+        <f t="shared" si="1"/>
         <v>666</v>
       </c>
     </row>
@@ -13622,14 +13622,14 @@
         <v>7675</v>
       </c>
       <c r="R160" s="1">
-        <f>((J160+K160+L160)*100)/D160</f>
+        <f t="shared" si="0"/>
         <v>40.248962655601659</v>
       </c>
       <c r="S160">
         <v>2020</v>
       </c>
       <c r="T160">
-        <f>(R160/100) * D160</f>
+        <f t="shared" si="1"/>
         <v>679</v>
       </c>
     </row>
@@ -13686,7 +13686,7 @@
         <v>8012</v>
       </c>
       <c r="R161" s="1">
-        <f>((J161+K161+L161)*100)/D161</f>
+        <f t="shared" si="0"/>
         <v>42.598870056497177</v>
       </c>
     </row>
@@ -13743,7 +13743,7 @@
         <v>8309</v>
       </c>
       <c r="R162" s="1">
-        <f>((J162+K162+L162)*100)/D162</f>
+        <f t="shared" si="0"/>
         <v>44.714131607335489</v>
       </c>
     </row>
@@ -13800,7 +13800,7 @@
         <v>8571</v>
       </c>
       <c r="R163" s="1">
-        <f>((J163+K163+L163)*100)/D163</f>
+        <f t="shared" si="0"/>
         <v>46.197327852004108</v>
       </c>
     </row>
@@ -13857,7 +13857,7 @@
         <v>8801</v>
       </c>
       <c r="R164" s="1">
-        <f>((J164+K164+L164)*100)/D164</f>
+        <f t="shared" si="0"/>
         <v>47.20314033366045</v>
       </c>
     </row>
@@ -13914,7 +13914,7 @@
         <v>8996</v>
       </c>
       <c r="R165" s="1">
-        <f>((J165+K165+L165)*100)/D165</f>
+        <f t="shared" si="0"/>
         <v>48.114985862393965</v>
       </c>
     </row>
@@ -13971,7 +13971,7 @@
         <v>9150</v>
       </c>
       <c r="R166" s="1">
-        <f>((J166+K166+L166)*100)/D166</f>
+        <f t="shared" si="0"/>
         <v>48.906107566089332</v>
       </c>
     </row>
@@ -14028,7 +14028,7 @@
         <v>9194</v>
       </c>
       <c r="R167" s="1">
-        <f>((J167+K167+L167)*100)/D167</f>
+        <f t="shared" si="0"/>
         <v>49.535603715170282</v>
       </c>
     </row>
@@ -14085,7 +14085,7 @@
         <v>9230</v>
       </c>
       <c r="R168" s="1">
-        <f>((J168+K168+L168)*100)/D168</f>
+        <f t="shared" si="0"/>
         <v>50.02148689299527</v>
       </c>
     </row>
@@ -14142,7 +14142,7 @@
         <v>9264</v>
       </c>
       <c r="R169" s="1">
-        <f>((J169+K169+L169)*100)/D169</f>
+        <f t="shared" si="0"/>
         <v>50.482990340193197</v>
       </c>
     </row>
@@ -14199,7 +14199,7 @@
         <v>9274</v>
       </c>
       <c r="R170" s="1">
-        <f>((J170+K170+L170)*100)/D170</f>
+        <f t="shared" si="0"/>
         <v>50.780608052588335</v>
       </c>
     </row>
@@ -14256,7 +14256,7 @@
         <v>9284</v>
       </c>
       <c r="R171" s="1">
-        <f>((J171+K171+L171)*100)/D171</f>
+        <f t="shared" si="0"/>
         <v>51.050080775444265</v>
       </c>
     </row>
@@ -14313,7 +14313,7 @@
         <v>9286</v>
       </c>
       <c r="R172" s="1">
-        <f>((J172+K172+L172)*100)/D172</f>
+        <f t="shared" si="0"/>
         <v>51.231135822081015</v>
       </c>
     </row>
@@ -14370,7 +14370,7 @@
         <v>9289</v>
       </c>
       <c r="R173" s="1">
-        <f>((J173+K173+L173)*100)/D173</f>
+        <f t="shared" si="0"/>
         <v>51.471165162808944</v>
       </c>
     </row>
@@ -14427,7 +14427,7 @@
         <v>9288</v>
       </c>
       <c r="R174" s="1">
-        <f>((J174+K174+L174)*100)/D174</f>
+        <f t="shared" si="0"/>
         <v>51.686700271423035</v>
       </c>
     </row>
@@ -14484,7 +14484,7 @@
         <v>9273</v>
       </c>
       <c r="R175" s="1">
-        <f>((J175+K175+L175)*100)/D175</f>
+        <f t="shared" si="0"/>
         <v>51.884615384615387</v>
       </c>
     </row>
@@ -14541,13 +14541,13 @@
         <v>9250</v>
       </c>
       <c r="R176" s="1">
-        <f>((J176+K176+L176)*100)/D176</f>
+        <f t="shared" si="0"/>
         <v>52.099236641221374</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{1A0EC4A6-A753-1F47-AC3A-00FE4B3C7C18}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1A0EC4A6-A753-1F47-AC3A-00FE4B3C7C18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15062,6 +15062,22 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="A4:A13"/>
     <mergeCell ref="B4:B13"/>
     <mergeCell ref="C4:C13"/>
@@ -15070,22 +15086,6 @@
     <mergeCell ref="B15:B22"/>
     <mergeCell ref="C15:C22"/>
     <mergeCell ref="D15:D22"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>